<commit_message>
Prepare diagrams and documentation for 2. milestone
</commit_message>
<xml_diff>
--- a/wykresyGantta.xlsx
+++ b/wykresyGantta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lara\Desktop\semestr 4\Inżynieria oprogramowania\lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE90DC7-B030-4A45-83F4-5CE240243011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE11195-B226-4763-913B-A9C65CC15882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HP-w" sheetId="10" r:id="rId1"/>
@@ -251,7 +251,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.32508271944751732"/>
+          <c:y val="0.10946344293461914"/>
+          <c:w val="0.65638020192813085"/>
+          <c:h val="0.84197817973248379"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -415,6 +425,438 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.3026076694803863E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0124264831373239E-17"/>
+                  <c:y val="2.3025252604331935E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.6745518389990926E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0124264831373239E-17"/>
+                  <c:y val="2.0932062805583049E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0024852966274648E-16"/>
+                  <c:y val="2.3025252604331952E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0024852966274648E-16"/>
+                  <c:y val="1.8838873006834143E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.883870818873987E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.3025087786237523E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.3820519546697754E-8"/>
+                  <c:y val="1.6745848026179781E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="1.5167375895533077E-2"/>
+                      <c:h val="3.367942386186925E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0024852966274648E-16"/>
+                  <c:y val="2.0931897987488658E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.0932062805583126E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.0931897987488658E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.7211467383735331E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.3025087786237523E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.8838708188739794E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.0931897987488658E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0024852966274648E-16"/>
+                  <c:y val="2.5118277584986391E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0024852966274648E-16"/>
+                  <c:y val="2.3025087786237523E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-A703-48AD-88DE-312C30358E1A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2588,6 +3030,138 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="4.1853675512697266E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-B08C-40FA-B4C2-243AC53C9B00}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3665201907662186E-3"/>
+                  <c:y val="4.1854005067899942E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-B08C-40FA-B4C2-243AC53C9B00}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3665201907662186E-3"/>
+                  <c:y val="4.3946351049452062E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-B08C-40FA-B4C2-243AC53C9B00}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0105161508993289E-17"/>
+                  <c:y val="4.1853510735096022E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-B08C-40FA-B4C2-243AC53C9B00}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="3.976083519834115E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-B08C-40FA-B4C2-243AC53C9B00}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="3.976083519834115E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-B08C-40FA-B4C2-243AC53C9B00}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2857,7 +3431,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5851,7 +6425,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A1A2B310-B7D0-4444-8485-35E7FD467D12}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5895,7 +6469,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CDF79628-490F-4EE2-80E2-7543269B94F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5906,7 +6480,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9303185" cy="6067295"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Wykres 1">
@@ -6038,7 +6612,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9303185" cy="6067295"/>
+    <xdr:ext cx="9293679" cy="6068786"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Wykres 1">
@@ -6413,7 +6987,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="0">$D3+$C3</f>
+        <f t="shared" ref="D4:D7" si="0">$D3+$C3</f>
         <v>5</v>
       </c>
       <c r="G4">

</xml_diff>